<commit_message>
updated data files with 2018 included: range now 2018-2023
</commit_message>
<xml_diff>
--- a/data/excel/Persone di 15 anni e più non andate in vacanza (IT1,68_161_DF_DCCV_TURANN_NO_TURAN_CAPI_1,1.0).xlsx
+++ b/data/excel/Persone di 15 anni e più non andate in vacanza (IT1,68_161_DF_DCCV_TURANN_NO_TURAN_CAPI_1,1.0).xlsx
@@ -22,17 +22,17 @@
         <t xml:space="preserve">Motivo della mancata vacanza: Il totale è riferito alle persone di 15 anni e più che non hanno effettuato vacanze.</t>
       </text>
     </comment>
-    <comment ref="S6" authorId="0">
+    <comment ref="R6" authorId="0">
       <text>
         <t xml:space="preserve">Motivo della mancata vacanza: Il totale è riferito alle persone di 15 anni e più che non hanno effettuato vacanze.</t>
       </text>
     </comment>
-    <comment ref="AB6" authorId="0">
+    <comment ref="AA6" authorId="0">
       <text>
         <t xml:space="preserve">Motivo della mancata vacanza: Il totale è riferito alle persone di 15 anni e più che non hanno effettuato vacanze.</t>
       </text>
     </comment>
-    <comment ref="AK6" authorId="0">
+    <comment ref="AJ6" authorId="0">
       <text>
         <t xml:space="preserve">Motivo della mancata vacanza: Il totale è riferito alle persone di 15 anni e più che non hanno effettuato vacanze.</t>
       </text>
@@ -42,12 +42,17 @@
         <t xml:space="preserve">Motivo della mancata vacanza: Il totale è riferito alle persone di 15 anni e più che non hanno effettuato vacanze.</t>
       </text>
     </comment>
+    <comment ref="BA6" authorId="0">
+      <text>
+        <t xml:space="preserve">Motivo della mancata vacanza: Il totale è riferito alle persone di 15 anni e più che non hanno effettuato vacanze.</t>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="34">
   <si>
     <t xml:space="preserve">Persone di 15 anni e più non andate in vacanza  </t>
   </si>
@@ -65,6 +70,9 @@
   </si>
   <si>
     <t xml:space="preserve">Motivo della mancata vacanza  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018  </t>
   </si>
   <si>
     <t xml:space="preserve">2019  </t>
@@ -371,7 +379,7 @@
         <v>7</v>
       </c>
       <c r="S5" s="4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="T5" s="4" t="s">
         <v>8</v>
@@ -398,7 +406,7 @@
         <v>8</v>
       </c>
       <c r="AB5" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="AC5" s="4" t="s">
         <v>9</v>
@@ -425,7 +433,7 @@
         <v>9</v>
       </c>
       <c r="AK5" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="AL5" s="4" t="s">
         <v>10</v>
@@ -450,6 +458,30 @@
       </c>
       <c r="AS5" s="4" t="s">
         <v>10</v>
+      </c>
+      <c r="AT5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="AU5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="AV5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="AW5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="AX5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="AY5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="AZ5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="BA5" s="4" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="6">
@@ -460,141 +492,165 @@
         <v>3</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D6" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="K6" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="L6" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="M6" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="N6" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="H6" s="4" t="s">
+      <c r="O6" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="I6" s="4" t="s">
+      <c r="P6" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="J6" s="4" t="s">
+      <c r="Q6" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="K6" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="L6" s="4" t="s">
+      <c r="R6" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="S6" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="M6" s="4" t="s">
+      <c r="T6" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="N6" s="4" t="s">
+      <c r="U6" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="O6" s="4" t="s">
+      <c r="V6" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="P6" s="4" t="s">
+      <c r="W6" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="Q6" s="4" t="s">
+      <c r="X6" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="Y6" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="Z6" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="AA6" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="R6" s="4" t="s">
+      <c r="AB6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="AC6" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="AE6" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="AF6" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="AG6" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="S6" s="4" t="s">
+      <c r="AH6" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="AI6" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="T6" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="U6" s="4" t="s">
+      <c r="AJ6" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="AK6" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="V6" s="4" t="s">
+      <c r="AL6" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="W6" s="4" t="s">
+      <c r="AM6" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="X6" s="4" t="s">
+      <c r="AN6" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="Y6" s="4" t="s">
+      <c r="AO6" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="Z6" s="4" t="s">
+      <c r="AP6" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="AQ6" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="AR6" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="AS6" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="AA6" s="4" t="s">
+      <c r="AT6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="AU6" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="AV6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="AW6" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="AX6" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="AY6" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="AB6" s="4" t="s">
+      <c r="AZ6" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="AC6" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="AD6" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="AE6" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AF6" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="AG6" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="AH6" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="AI6" s="4" t="s">
+      <c r="BA6" s="4" t="s">
         <v>19</v>
-      </c>
-      <c r="AJ6" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="AK6" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="AL6" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="AM6" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="AN6" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AO6" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="AP6" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="AQ6" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="AR6" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="AS6" s="4" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>3</v>
@@ -723,1376 +779,1640 @@
         <v>3</v>
       </c>
       <c r="AS7" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="AT7" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="AU7" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="AV7" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="AW7" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="AX7" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="AY7" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="AZ7" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="BA7" s="4" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C8" s="1">
+        <v>6270</v>
+      </c>
+      <c r="D8" s="1">
+        <v>3048</v>
+      </c>
+      <c r="E8" s="1">
+        <v>2436</v>
+      </c>
+      <c r="F8" s="1">
+        <v>1499</v>
+      </c>
+      <c r="G8" s="1">
+        <v>1476</v>
+      </c>
+      <c r="H8" s="1">
+        <v>217</v>
+      </c>
+      <c r="I8" s="1">
+        <v>353</v>
+      </c>
+      <c r="J8" s="1">
+        <v>13468</v>
+      </c>
+      <c r="K8" s="1">
         <v>5647</v>
       </c>
-      <c r="D8" s="1">
+      <c r="L8" s="1">
         <v>3170</v>
       </c>
-      <c r="E8" s="1">
+      <c r="M8" s="1">
         <v>2458</v>
       </c>
-      <c r="F8" s="1">
+      <c r="N8" s="1">
         <v>1641</v>
       </c>
-      <c r="G8" s="1">
+      <c r="O8" s="1">
         <v>1705</v>
       </c>
-      <c r="H8" s="1">
+      <c r="P8" s="1">
         <v>144</v>
       </c>
-      <c r="I8" s="1">
+      <c r="Q8" s="1">
         <v>559</v>
       </c>
-      <c r="J8" s="1">
+      <c r="R8" s="1">
         <v>13746</v>
       </c>
-      <c r="K8" s="1">
+      <c r="S8" s="1">
         <v>4907</v>
       </c>
-      <c r="L8" s="1">
+      <c r="T8" s="1">
         <v>2187</v>
       </c>
-      <c r="M8" s="1">
+      <c r="U8" s="1">
         <v>2221</v>
       </c>
-      <c r="N8" s="1">
+      <c r="V8" s="1">
         <v>1249</v>
       </c>
-      <c r="O8" s="1">
+      <c r="W8" s="1">
         <v>1289</v>
       </c>
-      <c r="P8" s="1">
+      <c r="X8" s="1">
         <v>215</v>
       </c>
-      <c r="Q8" s="1">
+      <c r="Y8" s="1">
         <v>9766</v>
       </c>
-      <c r="R8" s="1">
+      <c r="Z8" s="1">
         <v>406</v>
       </c>
-      <c r="S8" s="1">
+      <c r="AA8" s="1">
         <v>18445</v>
       </c>
-      <c r="T8" s="1">
+      <c r="AB8" s="1">
         <v>4879</v>
       </c>
-      <c r="U8" s="1">
+      <c r="AC8" s="1">
         <v>3181</v>
       </c>
-      <c r="V8" s="1">
+      <c r="AD8" s="1">
         <v>2538</v>
       </c>
-      <c r="W8" s="1">
+      <c r="AE8" s="1">
         <v>1422</v>
       </c>
-      <c r="X8" s="1">
+      <c r="AF8" s="1">
         <v>1336</v>
       </c>
-      <c r="Y8" s="1">
+      <c r="AG8" s="1">
         <v>219</v>
       </c>
-      <c r="Z8" s="1">
+      <c r="AH8" s="1">
         <v>5649</v>
       </c>
-      <c r="AA8" s="1">
+      <c r="AI8" s="1">
         <v>380</v>
       </c>
-      <c r="AB8" s="1">
+      <c r="AJ8" s="1">
         <v>16885</v>
       </c>
-      <c r="AC8" s="1">
+      <c r="AK8" s="1">
         <v>5138</v>
       </c>
-      <c r="AD8" s="1">
+      <c r="AL8" s="1">
         <v>3592</v>
       </c>
-      <c r="AE8" s="1">
+      <c r="AM8" s="1">
         <v>2713</v>
       </c>
-      <c r="AF8" s="1">
+      <c r="AN8" s="1">
         <v>1764</v>
       </c>
-      <c r="AG8" s="1">
+      <c r="AO8" s="1">
         <v>1358</v>
       </c>
-      <c r="AH8" s="1">
+      <c r="AP8" s="1">
         <v>252</v>
       </c>
-      <c r="AI8" s="1">
+      <c r="AQ8" s="1">
         <v>281</v>
       </c>
-      <c r="AJ8" s="1">
+      <c r="AR8" s="1">
         <v>432</v>
       </c>
-      <c r="AK8" s="1">
+      <c r="AS8" s="1">
         <v>14544</v>
       </c>
-      <c r="AL8" s="1">
+      <c r="AT8" s="1">
         <v>4683</v>
       </c>
-      <c r="AM8" s="1">
+      <c r="AU8" s="1">
         <v>4195</v>
       </c>
-      <c r="AN8" s="1">
+      <c r="AV8" s="1">
         <v>2620</v>
       </c>
-      <c r="AO8" s="1">
+      <c r="AW8" s="1">
         <v>1858</v>
       </c>
-      <c r="AP8" s="1">
+      <c r="AX8" s="1">
         <v>1187</v>
       </c>
-      <c r="AQ8" s="1">
+      <c r="AY8" s="1">
         <v>241</v>
       </c>
-      <c r="AR8" s="1">
+      <c r="AZ8" s="1">
         <v>610</v>
       </c>
-      <c r="AS8" s="1">
+      <c r="BA8" s="1">
         <v>14618</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="4" t="s">
-        <v>23</v>
-      </c>
       <c r="C9" s="1">
+        <v>6889</v>
+      </c>
+      <c r="D9" s="1">
+        <v>2408</v>
+      </c>
+      <c r="E9" s="1">
+        <v>3045</v>
+      </c>
+      <c r="F9" s="1">
+        <v>2219</v>
+      </c>
+      <c r="G9" s="1">
+        <v>2291</v>
+      </c>
+      <c r="H9" s="1">
+        <v>200</v>
+      </c>
+      <c r="I9" s="1">
+        <v>458</v>
+      </c>
+      <c r="J9" s="1">
+        <v>15205</v>
+      </c>
+      <c r="K9" s="1">
         <v>6214</v>
       </c>
-      <c r="D9" s="1">
+      <c r="L9" s="1">
         <v>2229</v>
       </c>
-      <c r="E9" s="1">
+      <c r="M9" s="1">
         <v>3064</v>
       </c>
-      <c r="F9" s="1">
+      <c r="N9" s="1">
         <v>2257</v>
       </c>
-      <c r="G9" s="1">
+      <c r="O9" s="1">
         <v>2405</v>
       </c>
-      <c r="H9" s="1">
+      <c r="P9" s="1">
         <v>212</v>
       </c>
-      <c r="I9" s="1">
+      <c r="Q9" s="1">
         <v>540</v>
       </c>
-      <c r="J9" s="1">
+      <c r="R9" s="1">
         <v>14904</v>
       </c>
-      <c r="K9" s="1">
+      <c r="S9" s="1">
         <v>5230</v>
       </c>
-      <c r="L9" s="1">
+      <c r="T9" s="1">
         <v>1549</v>
       </c>
-      <c r="M9" s="1">
+      <c r="U9" s="1">
         <v>2946</v>
       </c>
-      <c r="N9" s="1">
+      <c r="V9" s="1">
         <v>1756</v>
       </c>
-      <c r="O9" s="1">
+      <c r="W9" s="1">
         <v>1907</v>
       </c>
-      <c r="P9" s="1">
+      <c r="X9" s="1">
         <v>209</v>
       </c>
-      <c r="Q9" s="1">
+      <c r="Y9" s="1">
         <v>10659</v>
       </c>
-      <c r="R9" s="1">
+      <c r="Z9" s="1">
         <v>380</v>
       </c>
-      <c r="S9" s="1">
+      <c r="AA9" s="1">
         <v>20039</v>
       </c>
-      <c r="T9" s="1">
+      <c r="AB9" s="1">
         <v>5526</v>
       </c>
-      <c r="U9" s="1">
+      <c r="AC9" s="1">
         <v>2238</v>
       </c>
-      <c r="V9" s="1">
+      <c r="AD9" s="1">
         <v>3135</v>
       </c>
-      <c r="W9" s="1">
+      <c r="AE9" s="1">
         <v>1843</v>
       </c>
-      <c r="X9" s="1">
+      <c r="AF9" s="1">
         <v>1909</v>
       </c>
-      <c r="Y9" s="1">
+      <c r="AG9" s="1">
         <v>165</v>
       </c>
-      <c r="Z9" s="1">
+      <c r="AH9" s="1">
         <v>6344</v>
       </c>
-      <c r="AA9" s="1">
+      <c r="AI9" s="1">
         <v>421</v>
       </c>
-      <c r="AB9" s="1">
+      <c r="AJ9" s="1">
         <v>18382</v>
       </c>
-      <c r="AC9" s="1">
+      <c r="AK9" s="1">
         <v>5495</v>
       </c>
-      <c r="AD9" s="1">
+      <c r="AL9" s="1">
         <v>2517</v>
       </c>
-      <c r="AE9" s="1">
+      <c r="AM9" s="1">
         <v>3427</v>
       </c>
-      <c r="AF9" s="1">
+      <c r="AN9" s="1">
         <v>2512</v>
       </c>
-      <c r="AG9" s="1">
+      <c r="AO9" s="1">
         <v>1915</v>
       </c>
-      <c r="AH9" s="1">
+      <c r="AP9" s="1">
         <v>251</v>
       </c>
-      <c r="AI9" s="1">
+      <c r="AQ9" s="1">
         <v>339</v>
       </c>
-      <c r="AJ9" s="1">
+      <c r="AR9" s="1">
         <v>504</v>
       </c>
-      <c r="AK9" s="1">
+      <c r="AS9" s="1">
         <v>15753</v>
       </c>
-      <c r="AL9" s="1">
+      <c r="AT9" s="1">
         <v>5056</v>
       </c>
-      <c r="AM9" s="1">
+      <c r="AU9" s="1">
         <v>3124</v>
       </c>
-      <c r="AN9" s="1">
+      <c r="AV9" s="1">
         <v>3134</v>
       </c>
-      <c r="AO9" s="1">
+      <c r="AW9" s="1">
         <v>2760</v>
       </c>
-      <c r="AP9" s="1">
+      <c r="AX9" s="1">
         <v>2012</v>
       </c>
-      <c r="AQ9" s="1">
+      <c r="AY9" s="1">
         <v>273</v>
       </c>
-      <c r="AR9" s="1">
+      <c r="AZ9" s="1">
         <v>714</v>
       </c>
-      <c r="AS9" s="1">
+      <c r="BA9" s="1">
         <v>16067</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C10" s="1">
+        <v>1502</v>
+      </c>
+      <c r="D10" s="1">
+        <v>1147</v>
+      </c>
+      <c r="E10" s="1">
+        <v>217</v>
+      </c>
+      <c r="F10" s="1">
+        <v>301</v>
+      </c>
+      <c r="G10" s="1">
+        <v>14</v>
+      </c>
+      <c r="H10" s="1">
+        <v>43</v>
+      </c>
+      <c r="I10" s="1">
+        <v>79</v>
+      </c>
+      <c r="J10" s="1">
+        <v>3011</v>
+      </c>
+      <c r="K10" s="1">
         <v>1574</v>
       </c>
-      <c r="D10" s="1">
+      <c r="L10" s="1">
         <v>1098</v>
       </c>
-      <c r="E10" s="1">
+      <c r="M10" s="1">
         <v>249</v>
       </c>
-      <c r="F10" s="1">
+      <c r="N10" s="1">
         <v>345</v>
       </c>
-      <c r="G10" s="1">
+      <c r="O10" s="1">
         <v>37</v>
       </c>
-      <c r="H10" s="1">
+      <c r="P10" s="1">
         <v>28</v>
       </c>
-      <c r="I10" s="1">
+      <c r="Q10" s="1">
         <v>99</v>
       </c>
-      <c r="J10" s="1">
+      <c r="R10" s="1">
         <v>3063</v>
       </c>
-      <c r="K10" s="1">
+      <c r="S10" s="1">
         <v>1558</v>
       </c>
-      <c r="L10" s="1">
+      <c r="T10" s="1">
         <v>705</v>
       </c>
-      <c r="M10" s="1">
+      <c r="U10" s="1">
         <v>172</v>
       </c>
-      <c r="N10" s="1">
+      <c r="V10" s="1">
         <v>320</v>
       </c>
-      <c r="O10" s="1">
+      <c r="W10" s="1">
         <v>36</v>
       </c>
-      <c r="P10" s="1">
+      <c r="X10" s="1">
         <v>54</v>
       </c>
-      <c r="Q10" s="1">
+      <c r="Y10" s="1">
         <v>2347</v>
       </c>
-      <c r="R10" s="1">
+      <c r="Z10" s="1">
         <v>98</v>
       </c>
-      <c r="S10" s="1">
+      <c r="AA10" s="1">
         <v>4411</v>
       </c>
-      <c r="T10" s="1">
+      <c r="AB10" s="1">
         <v>1444</v>
       </c>
-      <c r="U10" s="1">
+      <c r="AC10" s="1">
         <v>1004</v>
       </c>
-      <c r="V10" s="1">
+      <c r="AD10" s="1">
         <v>237</v>
       </c>
-      <c r="W10" s="1">
+      <c r="AE10" s="1">
         <v>248</v>
       </c>
-      <c r="X10" s="1">
+      <c r="AF10" s="1">
         <v>43</v>
       </c>
-      <c r="Y10" s="1">
+      <c r="AG10" s="1">
         <v>53</v>
       </c>
-      <c r="Z10" s="1">
+      <c r="AH10" s="1">
         <v>1196</v>
       </c>
-      <c r="AA10" s="1">
+      <c r="AI10" s="1">
         <v>97</v>
       </c>
-      <c r="AB10" s="1">
+      <c r="AJ10" s="1">
         <v>3808</v>
       </c>
-      <c r="AC10" s="1">
+      <c r="AK10" s="1">
         <v>1527</v>
       </c>
-      <c r="AD10" s="1">
+      <c r="AL10" s="1">
         <v>1153</v>
       </c>
-      <c r="AE10" s="1">
+      <c r="AM10" s="1">
         <v>224</v>
       </c>
-      <c r="AF10" s="1">
+      <c r="AN10" s="1">
         <v>409</v>
       </c>
-      <c r="AG10" s="1">
+      <c r="AO10" s="1">
         <v>52</v>
       </c>
-      <c r="AH10" s="1">
+      <c r="AP10" s="1">
         <v>32</v>
       </c>
-      <c r="AI10" s="1">
+      <c r="AQ10" s="1">
         <v>29</v>
       </c>
-      <c r="AJ10" s="1">
+      <c r="AR10" s="1">
         <v>98</v>
       </c>
-      <c r="AK10" s="1">
+      <c r="AS10" s="1">
         <v>3355</v>
       </c>
-      <c r="AL10" s="1">
+      <c r="AT10" s="1">
         <v>1106</v>
       </c>
-      <c r="AM10" s="1">
+      <c r="AU10" s="1">
         <v>1447</v>
       </c>
-      <c r="AN10" s="1">
+      <c r="AV10" s="1">
         <v>191</v>
       </c>
-      <c r="AO10" s="1">
+      <c r="AW10" s="1">
         <v>343</v>
       </c>
-      <c r="AP10" s="1">
+      <c r="AX10" s="1">
         <v>30</v>
       </c>
-      <c r="AQ10" s="1">
+      <c r="AY10" s="1">
         <v>53</v>
       </c>
-      <c r="AR10" s="1">
+      <c r="AZ10" s="1">
         <v>124</v>
       </c>
-      <c r="AS10" s="1">
+      <c r="BA10" s="1">
         <v>3217</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C11" s="1">
+        <v>1735</v>
+      </c>
+      <c r="D11" s="1">
+        <v>939</v>
+      </c>
+      <c r="E11" s="1">
+        <v>236</v>
+      </c>
+      <c r="F11" s="1">
+        <v>315</v>
+      </c>
+      <c r="G11" s="1">
+        <v>63</v>
+      </c>
+      <c r="H11" s="1">
+        <v>14</v>
+      </c>
+      <c r="I11" s="1">
+        <v>24</v>
+      </c>
+      <c r="J11" s="1">
+        <v>3046</v>
+      </c>
+      <c r="K11" s="1">
         <v>1545</v>
       </c>
-      <c r="D11" s="1">
+      <c r="L11" s="1">
         <v>858</v>
       </c>
-      <c r="E11" s="1">
+      <c r="M11" s="1">
         <v>240</v>
       </c>
-      <c r="F11" s="1">
+      <c r="N11" s="1">
         <v>309</v>
       </c>
-      <c r="G11" s="1">
+      <c r="O11" s="1">
         <v>75</v>
       </c>
-      <c r="H11" s="1">
+      <c r="P11" s="1">
         <v>48</v>
       </c>
-      <c r="I11" s="1">
+      <c r="Q11" s="1">
         <v>86</v>
       </c>
-      <c r="J11" s="1">
+      <c r="R11" s="1">
         <v>2749</v>
       </c>
-      <c r="K11" s="1">
+      <c r="S11" s="1">
         <v>1393</v>
       </c>
-      <c r="L11" s="1">
+      <c r="T11" s="1">
         <v>609</v>
       </c>
-      <c r="M11" s="1">
+      <c r="U11" s="1">
         <v>205</v>
       </c>
-      <c r="N11" s="1">
+      <c r="V11" s="1">
         <v>286</v>
       </c>
-      <c r="O11" s="1">
+      <c r="W11" s="1">
         <v>70</v>
       </c>
-      <c r="P11" s="1">
+      <c r="X11" s="1">
         <v>47</v>
       </c>
-      <c r="Q11" s="1">
+      <c r="Y11" s="1">
         <v>2162</v>
       </c>
-      <c r="R11" s="1">
+      <c r="Z11" s="1">
         <v>111</v>
       </c>
-      <c r="S11" s="1">
+      <c r="AA11" s="1">
         <v>4059</v>
       </c>
-      <c r="T11" s="1">
+      <c r="AB11" s="1">
         <v>1422</v>
       </c>
-      <c r="U11" s="1">
+      <c r="AC11" s="1">
         <v>1031</v>
       </c>
-      <c r="V11" s="1">
+      <c r="AD11" s="1">
         <v>152</v>
       </c>
-      <c r="W11" s="1">
+      <c r="AE11" s="1">
         <v>275</v>
       </c>
-      <c r="X11" s="1">
+      <c r="AF11" s="1">
         <v>38</v>
       </c>
-      <c r="Y11" s="1">
+      <c r="AG11" s="1">
         <v>36</v>
       </c>
-      <c r="Z11" s="1">
+      <c r="AH11" s="1">
         <v>1243</v>
       </c>
-      <c r="AA11" s="1">
+      <c r="AI11" s="1">
         <v>76</v>
       </c>
-      <c r="AB11" s="1">
+      <c r="AJ11" s="1">
         <v>3737</v>
       </c>
-      <c r="AC11" s="1">
+      <c r="AK11" s="1">
         <v>1024</v>
       </c>
-      <c r="AD11" s="1">
+      <c r="AL11" s="1">
         <v>895</v>
       </c>
-      <c r="AE11" s="1">
+      <c r="AM11" s="1">
         <v>194</v>
       </c>
-      <c r="AF11" s="1">
+      <c r="AN11" s="1">
         <v>271</v>
       </c>
-      <c r="AG11" s="1">
+      <c r="AO11" s="1">
         <v>64</v>
       </c>
-      <c r="AH11" s="1">
+      <c r="AP11" s="1">
         <v>74</v>
       </c>
-      <c r="AI11" s="1">
+      <c r="AQ11" s="1">
         <v>49</v>
       </c>
-      <c r="AJ11" s="1">
+      <c r="AR11" s="1">
         <v>79</v>
       </c>
-      <c r="AK11" s="1">
+      <c r="AS11" s="1">
         <v>2496</v>
       </c>
-      <c r="AL11" s="1">
+      <c r="AT11" s="1">
         <v>1361</v>
       </c>
-      <c r="AM11" s="1">
+      <c r="AU11" s="1">
         <v>1069</v>
       </c>
-      <c r="AN11" s="1">
+      <c r="AV11" s="1">
         <v>206</v>
       </c>
-      <c r="AO11" s="1">
+      <c r="AW11" s="1">
         <v>340</v>
       </c>
-      <c r="AP11" s="1">
+      <c r="AX11" s="1">
         <v>31</v>
       </c>
-      <c r="AQ11" s="1">
+      <c r="AY11" s="1">
         <v>33</v>
       </c>
-      <c r="AR11" s="1">
+      <c r="AZ11" s="1">
         <v>68</v>
       </c>
-      <c r="AS11" s="1">
+      <c r="BA11" s="1">
         <v>2950</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C12" s="1">
+        <v>3236</v>
+      </c>
+      <c r="D12" s="1">
+        <v>2087</v>
+      </c>
+      <c r="E12" s="1">
+        <v>452</v>
+      </c>
+      <c r="F12" s="1">
+        <v>616</v>
+      </c>
+      <c r="G12" s="1">
+        <v>77</v>
+      </c>
+      <c r="H12" s="1">
+        <v>57</v>
+      </c>
+      <c r="I12" s="1">
+        <v>103</v>
+      </c>
+      <c r="J12" s="1">
+        <v>6057</v>
+      </c>
+      <c r="K12" s="1">
         <v>3119</v>
       </c>
-      <c r="D12" s="1">
+      <c r="L12" s="1">
         <v>1956</v>
       </c>
-      <c r="E12" s="1">
+      <c r="M12" s="1">
         <v>489</v>
       </c>
-      <c r="F12" s="1">
+      <c r="N12" s="1">
         <v>654</v>
       </c>
-      <c r="G12" s="1">
+      <c r="O12" s="1">
         <v>113</v>
       </c>
-      <c r="H12" s="1">
+      <c r="P12" s="1">
         <v>75</v>
       </c>
-      <c r="I12" s="1">
+      <c r="Q12" s="1">
         <v>185</v>
       </c>
-      <c r="J12" s="1">
+      <c r="R12" s="1">
         <v>5813</v>
       </c>
-      <c r="K12" s="1">
+      <c r="S12" s="1">
         <v>2950</v>
       </c>
-      <c r="L12" s="1">
+      <c r="T12" s="1">
         <v>1313</v>
       </c>
-      <c r="M12" s="1">
+      <c r="U12" s="1">
         <v>376</v>
       </c>
-      <c r="N12" s="1">
+      <c r="V12" s="1">
         <v>607</v>
       </c>
-      <c r="O12" s="1">
+      <c r="W12" s="1">
         <v>107</v>
       </c>
-      <c r="P12" s="1">
+      <c r="X12" s="1">
         <v>101</v>
       </c>
-      <c r="Q12" s="1">
+      <c r="Y12" s="1">
         <v>4510</v>
       </c>
-      <c r="R12" s="1">
+      <c r="Z12" s="1">
         <v>209</v>
       </c>
-      <c r="S12" s="1">
+      <c r="AA12" s="1">
         <v>8470</v>
       </c>
-      <c r="T12" s="1">
+      <c r="AB12" s="1">
         <v>2866</v>
       </c>
-      <c r="U12" s="1">
+      <c r="AC12" s="1">
         <v>2035</v>
       </c>
-      <c r="V12" s="1">
+      <c r="AD12" s="1">
         <v>389</v>
       </c>
-      <c r="W12" s="1">
+      <c r="AE12" s="1">
         <v>522</v>
       </c>
-      <c r="X12" s="1">
+      <c r="AF12" s="1">
         <v>80</v>
       </c>
-      <c r="Y12" s="1">
+      <c r="AG12" s="1">
         <v>89</v>
       </c>
-      <c r="Z12" s="1">
+      <c r="AH12" s="1">
         <v>2438</v>
       </c>
-      <c r="AA12" s="1">
+      <c r="AI12" s="1">
         <v>172</v>
       </c>
-      <c r="AB12" s="1">
+      <c r="AJ12" s="1">
         <v>7546</v>
       </c>
-      <c r="AC12" s="1">
+      <c r="AK12" s="1">
         <v>2552</v>
       </c>
-      <c r="AD12" s="1">
+      <c r="AL12" s="1">
         <v>2048</v>
       </c>
-      <c r="AE12" s="1">
+      <c r="AM12" s="1">
         <v>418</v>
       </c>
-      <c r="AF12" s="1">
+      <c r="AN12" s="1">
         <v>680</v>
       </c>
-      <c r="AG12" s="1">
+      <c r="AO12" s="1">
         <v>116</v>
       </c>
-      <c r="AH12" s="1">
+      <c r="AP12" s="1">
         <v>106</v>
       </c>
-      <c r="AI12" s="1">
+      <c r="AQ12" s="1">
         <v>78</v>
       </c>
-      <c r="AJ12" s="1">
+      <c r="AR12" s="1">
         <v>176</v>
       </c>
-      <c r="AK12" s="1">
+      <c r="AS12" s="1">
         <v>5852</v>
       </c>
-      <c r="AL12" s="1">
+      <c r="AT12" s="1">
         <v>2468</v>
       </c>
-      <c r="AM12" s="1">
+      <c r="AU12" s="1">
         <v>2516</v>
       </c>
-      <c r="AN12" s="1">
+      <c r="AV12" s="1">
         <v>396</v>
       </c>
-      <c r="AO12" s="1">
+      <c r="AW12" s="1">
         <v>684</v>
       </c>
-      <c r="AP12" s="1">
+      <c r="AX12" s="1">
         <v>62</v>
       </c>
-      <c r="AQ12" s="1">
+      <c r="AY12" s="1">
         <v>86</v>
       </c>
-      <c r="AR12" s="1">
+      <c r="AZ12" s="1">
         <v>192</v>
       </c>
-      <c r="AS12" s="1">
+      <c r="BA12" s="1">
         <v>6167</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C13" s="1">
+        <v>2134</v>
+      </c>
+      <c r="D13" s="1">
+        <v>1095</v>
+      </c>
+      <c r="E13" s="1">
+        <v>238</v>
+      </c>
+      <c r="F13" s="1">
+        <v>441</v>
+      </c>
+      <c r="G13" s="1">
+        <v>72</v>
+      </c>
+      <c r="H13" s="1">
+        <v>41</v>
+      </c>
+      <c r="I13" s="1">
+        <v>59</v>
+      </c>
+      <c r="J13" s="1">
+        <v>3675</v>
+      </c>
+      <c r="K13" s="1">
         <v>1998</v>
       </c>
-      <c r="D13" s="1">
+      <c r="L13" s="1">
         <v>1061</v>
       </c>
-      <c r="E13" s="1">
+      <c r="M13" s="1">
         <v>273</v>
       </c>
-      <c r="F13" s="1">
+      <c r="N13" s="1">
         <v>525</v>
       </c>
-      <c r="G13" s="1">
+      <c r="O13" s="1">
         <v>101</v>
       </c>
-      <c r="H13" s="1">
+      <c r="P13" s="1">
         <v>65</v>
       </c>
-      <c r="I13" s="1">
+      <c r="Q13" s="1">
         <v>104</v>
       </c>
-      <c r="J13" s="1">
+      <c r="R13" s="1">
         <v>3672</v>
       </c>
-      <c r="K13" s="1">
+      <c r="S13" s="1">
         <v>1481</v>
       </c>
-      <c r="L13" s="1">
+      <c r="T13" s="1">
         <v>876</v>
       </c>
-      <c r="M13" s="1">
+      <c r="U13" s="1">
         <v>272</v>
       </c>
-      <c r="N13" s="1">
+      <c r="V13" s="1">
         <v>404</v>
       </c>
-      <c r="O13" s="1">
+      <c r="W13" s="1">
         <v>66</v>
       </c>
-      <c r="P13" s="1">
+      <c r="X13" s="1">
         <v>52</v>
       </c>
-      <c r="Q13" s="1">
+      <c r="Y13" s="1">
         <v>3078</v>
       </c>
-      <c r="R13" s="1">
+      <c r="Z13" s="1">
         <v>122</v>
       </c>
-      <c r="S13" s="1">
+      <c r="AA13" s="1">
         <v>5183</v>
       </c>
-      <c r="T13" s="1">
+      <c r="AB13" s="1">
         <v>1612</v>
       </c>
-      <c r="U13" s="1">
+      <c r="AC13" s="1">
         <v>873</v>
       </c>
-      <c r="V13" s="1">
+      <c r="AD13" s="1">
         <v>325</v>
       </c>
-      <c r="W13" s="1">
+      <c r="AE13" s="1">
         <v>439</v>
       </c>
-      <c r="X13" s="1">
+      <c r="AF13" s="1">
         <v>99</v>
       </c>
-      <c r="Y13" s="1">
+      <c r="AG13" s="1">
         <v>34</v>
       </c>
-      <c r="Z13" s="1">
+      <c r="AH13" s="1">
         <v>1523</v>
       </c>
-      <c r="AA13" s="1">
+      <c r="AI13" s="1">
         <v>112</v>
       </c>
-      <c r="AB13" s="1">
+      <c r="AJ13" s="1">
         <v>4369</v>
       </c>
-      <c r="AC13" s="1">
+      <c r="AK13" s="1">
         <v>1695</v>
       </c>
-      <c r="AD13" s="1">
+      <c r="AL13" s="1">
         <v>1204</v>
       </c>
-      <c r="AE13" s="1">
+      <c r="AM13" s="1">
         <v>308</v>
       </c>
-      <c r="AF13" s="1">
+      <c r="AN13" s="1">
         <v>443</v>
       </c>
-      <c r="AG13" s="1">
+      <c r="AO13" s="1">
         <v>81</v>
       </c>
-      <c r="AH13" s="1">
+      <c r="AP13" s="1">
         <v>60</v>
       </c>
-      <c r="AI13" s="1">
+      <c r="AQ13" s="1">
         <v>84</v>
       </c>
-      <c r="AJ13" s="1">
+      <c r="AR13" s="1">
         <v>140</v>
       </c>
-      <c r="AK13" s="1">
+      <c r="AS13" s="1">
         <v>3788</v>
       </c>
-      <c r="AL13" s="1">
+      <c r="AT13" s="1">
         <v>1492</v>
       </c>
-      <c r="AM13" s="1">
+      <c r="AU13" s="1">
         <v>1224</v>
       </c>
-      <c r="AN13" s="1">
+      <c r="AV13" s="1">
         <v>207</v>
       </c>
-      <c r="AO13" s="1">
+      <c r="AW13" s="1">
         <v>504</v>
       </c>
-      <c r="AP13" s="1">
+      <c r="AX13" s="1">
         <v>57</v>
       </c>
-      <c r="AQ13" s="1">
+      <c r="AY13" s="1">
         <v>66</v>
       </c>
-      <c r="AR13" s="1">
+      <c r="AZ13" s="1">
         <v>213</v>
       </c>
-      <c r="AS13" s="1">
+      <c r="BA13" s="1">
         <v>3619</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C14" s="1">
+        <v>2678</v>
+      </c>
+      <c r="D14" s="1">
+        <v>1267</v>
+      </c>
+      <c r="E14" s="1">
+        <v>585</v>
+      </c>
+      <c r="F14" s="1">
+        <v>581</v>
+      </c>
+      <c r="G14" s="1">
+        <v>144</v>
+      </c>
+      <c r="H14" s="1">
+        <v>79</v>
+      </c>
+      <c r="I14" s="1">
+        <v>139</v>
+      </c>
+      <c r="J14" s="1">
+        <v>4835</v>
+      </c>
+      <c r="K14" s="1">
         <v>2400</v>
       </c>
-      <c r="D14" s="1">
+      <c r="L14" s="1">
         <v>1348</v>
       </c>
-      <c r="E14" s="1">
+      <c r="M14" s="1">
         <v>528</v>
       </c>
-      <c r="F14" s="1">
+      <c r="N14" s="1">
         <v>708</v>
       </c>
-      <c r="G14" s="1">
+      <c r="O14" s="1">
         <v>272</v>
       </c>
-      <c r="H14" s="1">
+      <c r="P14" s="1">
         <v>92</v>
       </c>
-      <c r="I14" s="1">
+      <c r="Q14" s="1">
         <v>176</v>
       </c>
-      <c r="J14" s="1">
+      <c r="R14" s="1">
         <v>4920</v>
       </c>
-      <c r="K14" s="1">
+      <c r="S14" s="1">
         <v>2100</v>
       </c>
-      <c r="L14" s="1">
+      <c r="T14" s="1">
         <v>767</v>
       </c>
-      <c r="M14" s="1">
+      <c r="U14" s="1">
         <v>562</v>
       </c>
-      <c r="N14" s="1">
+      <c r="V14" s="1">
         <v>494</v>
       </c>
-      <c r="O14" s="1">
+      <c r="W14" s="1">
         <v>207</v>
       </c>
-      <c r="P14" s="1">
+      <c r="X14" s="1">
         <v>54</v>
       </c>
-      <c r="Q14" s="1">
+      <c r="Y14" s="1">
         <v>3672</v>
       </c>
-      <c r="R14" s="1">
+      <c r="Z14" s="1">
         <v>147</v>
       </c>
-      <c r="S14" s="1">
+      <c r="AA14" s="1">
         <v>6478</v>
       </c>
-      <c r="T14" s="1">
+      <c r="AB14" s="1">
         <v>2186</v>
       </c>
-      <c r="U14" s="1">
+      <c r="AC14" s="1">
         <v>1456</v>
       </c>
-      <c r="V14" s="1">
+      <c r="AD14" s="1">
         <v>680</v>
       </c>
-      <c r="W14" s="1">
+      <c r="AE14" s="1">
         <v>561</v>
       </c>
-      <c r="X14" s="1">
+      <c r="AF14" s="1">
         <v>160</v>
       </c>
-      <c r="Y14" s="1">
+      <c r="AG14" s="1">
         <v>75</v>
       </c>
-      <c r="Z14" s="1">
+      <c r="AH14" s="1">
         <v>2024</v>
       </c>
-      <c r="AA14" s="1">
+      <c r="AI14" s="1">
         <v>104</v>
       </c>
-      <c r="AB14" s="1">
+      <c r="AJ14" s="1">
         <v>6131</v>
       </c>
-      <c r="AC14" s="1">
+      <c r="AK14" s="1">
         <v>2025</v>
       </c>
-      <c r="AD14" s="1">
+      <c r="AL14" s="1">
         <v>1529</v>
       </c>
-      <c r="AE14" s="1">
+      <c r="AM14" s="1">
         <v>505</v>
       </c>
-      <c r="AF14" s="1">
+      <c r="AN14" s="1">
         <v>622</v>
       </c>
-      <c r="AG14" s="1">
+      <c r="AO14" s="1">
         <v>125</v>
       </c>
-      <c r="AH14" s="1">
+      <c r="AP14" s="1">
         <v>52</v>
       </c>
-      <c r="AI14" s="1">
+      <c r="AQ14" s="1">
         <v>65</v>
       </c>
-      <c r="AJ14" s="1">
+      <c r="AR14" s="1">
         <v>159</v>
       </c>
-      <c r="AK14" s="1">
+      <c r="AS14" s="1">
         <v>4777</v>
       </c>
-      <c r="AL14" s="1">
+      <c r="AT14" s="1">
         <v>1614</v>
       </c>
-      <c r="AM14" s="1">
+      <c r="AU14" s="1">
         <v>1775</v>
       </c>
-      <c r="AN14" s="1">
+      <c r="AV14" s="1">
         <v>590</v>
       </c>
-      <c r="AO14" s="1">
+      <c r="AW14" s="1">
         <v>584</v>
       </c>
-      <c r="AP14" s="1">
+      <c r="AX14" s="1">
         <v>161</v>
       </c>
-      <c r="AQ14" s="1">
+      <c r="AY14" s="1">
         <v>74</v>
       </c>
-      <c r="AR14" s="1">
+      <c r="AZ14" s="1">
         <v>180</v>
       </c>
-      <c r="AS14" s="1">
+      <c r="BA14" s="1">
         <v>4765</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C15" s="1">
+        <v>2221</v>
+      </c>
+      <c r="D15" s="1">
+        <v>741</v>
+      </c>
+      <c r="E15" s="1">
+        <v>807</v>
+      </c>
+      <c r="F15" s="1">
+        <v>518</v>
+      </c>
+      <c r="G15" s="1">
+        <v>283</v>
+      </c>
+      <c r="H15" s="1">
+        <v>73</v>
+      </c>
+      <c r="I15" s="1">
+        <v>100</v>
+      </c>
+      <c r="J15" s="1">
+        <v>4146</v>
+      </c>
+      <c r="K15" s="1">
         <v>2038</v>
       </c>
-      <c r="D15" s="1">
+      <c r="L15" s="1">
         <v>858</v>
       </c>
-      <c r="E15" s="1">
+      <c r="M15" s="1">
         <v>880</v>
       </c>
-      <c r="F15" s="1">
+      <c r="N15" s="1">
         <v>667</v>
       </c>
-      <c r="G15" s="1">
+      <c r="O15" s="1">
         <v>362</v>
       </c>
-      <c r="H15" s="1">
+      <c r="P15" s="1">
         <v>45</v>
       </c>
-      <c r="I15" s="1">
+      <c r="Q15" s="1">
         <v>232</v>
       </c>
-      <c r="J15" s="1">
+      <c r="R15" s="1">
         <v>4464</v>
       </c>
-      <c r="K15" s="1">
+      <c r="S15" s="1">
         <v>1800</v>
       </c>
-      <c r="L15" s="1">
+      <c r="T15" s="1">
         <v>618</v>
       </c>
-      <c r="M15" s="1">
+      <c r="U15" s="1">
         <v>797</v>
       </c>
-      <c r="N15" s="1">
+      <c r="V15" s="1">
         <v>525</v>
       </c>
-      <c r="O15" s="1">
+      <c r="W15" s="1">
         <v>319</v>
       </c>
-      <c r="P15" s="1">
+      <c r="X15" s="1">
         <v>81</v>
       </c>
-      <c r="Q15" s="1">
+      <c r="Y15" s="1">
         <v>3609</v>
       </c>
-      <c r="R15" s="1">
+      <c r="Z15" s="1">
         <v>100</v>
       </c>
-      <c r="S15" s="1">
+      <c r="AA15" s="1">
         <v>6489</v>
       </c>
-      <c r="T15" s="1">
+      <c r="AB15" s="1">
         <v>1802</v>
       </c>
-      <c r="U15" s="1">
+      <c r="AC15" s="1">
         <v>835</v>
       </c>
-      <c r="V15" s="1">
+      <c r="AD15" s="1">
         <v>846</v>
       </c>
-      <c r="W15" s="1">
+      <c r="AE15" s="1">
         <v>510</v>
       </c>
-      <c r="X15" s="1">
+      <c r="AF15" s="1">
         <v>276</v>
       </c>
-      <c r="Y15" s="1">
+      <c r="AG15" s="1">
         <v>81</v>
       </c>
-      <c r="Z15" s="1">
+      <c r="AH15" s="1">
         <v>2000</v>
       </c>
-      <c r="AA15" s="1">
+      <c r="AI15" s="1">
         <v>147</v>
       </c>
-      <c r="AB15" s="1">
+      <c r="AJ15" s="1">
         <v>5677</v>
       </c>
-      <c r="AC15" s="1">
+      <c r="AK15" s="1">
         <v>2011</v>
       </c>
-      <c r="AD15" s="1">
+      <c r="AL15" s="1">
         <v>1053</v>
       </c>
-      <c r="AE15" s="1">
+      <c r="AM15" s="1">
         <v>958</v>
       </c>
-      <c r="AF15" s="1">
+      <c r="AN15" s="1">
         <v>898</v>
       </c>
-      <c r="AG15" s="1">
+      <c r="AO15" s="1">
         <v>301</v>
       </c>
-      <c r="AH15" s="1">
+      <c r="AP15" s="1">
         <v>114</v>
       </c>
-      <c r="AI15" s="1">
+      <c r="AQ15" s="1">
         <v>88</v>
       </c>
-      <c r="AJ15" s="1">
+      <c r="AR15" s="1">
         <v>167</v>
       </c>
-      <c r="AK15" s="1">
+      <c r="AS15" s="1">
         <v>5250</v>
       </c>
-      <c r="AL15" s="1">
+      <c r="AT15" s="1">
         <v>1896</v>
       </c>
-      <c r="AM15" s="1">
+      <c r="AU15" s="1">
         <v>1453</v>
       </c>
-      <c r="AN15" s="1">
+      <c r="AV15" s="1">
         <v>950</v>
       </c>
-      <c r="AO15" s="1">
+      <c r="AW15" s="1">
         <v>982</v>
       </c>
-      <c r="AP15" s="1">
+      <c r="AX15" s="1">
         <v>229</v>
       </c>
-      <c r="AQ15" s="1">
+      <c r="AY15" s="1">
         <v>117</v>
       </c>
-      <c r="AR15" s="1">
+      <c r="AZ15" s="1">
         <v>205</v>
       </c>
-      <c r="AS15" s="1">
+      <c r="BA15" s="1">
         <v>5522</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C16" s="1">
+        <v>2889</v>
+      </c>
+      <c r="D16" s="1">
+        <v>266</v>
+      </c>
+      <c r="E16" s="1">
+        <v>3398</v>
+      </c>
+      <c r="F16" s="1">
+        <v>1563</v>
+      </c>
+      <c r="G16" s="1">
+        <v>3191</v>
+      </c>
+      <c r="H16" s="1">
+        <v>167</v>
+      </c>
+      <c r="I16" s="1">
+        <v>410</v>
+      </c>
+      <c r="J16" s="1">
+        <v>9960</v>
+      </c>
+      <c r="K16" s="1">
         <v>2307</v>
       </c>
-      <c r="D16" s="1">
+      <c r="L16" s="1">
         <v>175</v>
       </c>
-      <c r="E16" s="1">
+      <c r="M16" s="1">
         <v>3352</v>
       </c>
-      <c r="F16" s="1">
+      <c r="N16" s="1">
         <v>1344</v>
       </c>
-      <c r="G16" s="1">
+      <c r="O16" s="1">
         <v>3262</v>
       </c>
-      <c r="H16" s="1">
+      <c r="P16" s="1">
         <v>79</v>
       </c>
-      <c r="I16" s="1">
+      <c r="Q16" s="1">
         <v>403</v>
       </c>
-      <c r="J16" s="1">
+      <c r="R16" s="1">
         <v>9781</v>
       </c>
-      <c r="K16" s="1">
+      <c r="S16" s="1">
         <v>1806</v>
       </c>
-      <c r="L16" s="1">
+      <c r="T16" s="1">
         <v>162</v>
       </c>
-      <c r="M16" s="1">
+      <c r="U16" s="1">
         <v>3159</v>
       </c>
-      <c r="N16" s="1">
+      <c r="V16" s="1">
         <v>976</v>
       </c>
-      <c r="O16" s="1">
+      <c r="W16" s="1">
         <v>2497</v>
       </c>
-      <c r="P16" s="1">
+      <c r="X16" s="1">
         <v>135</v>
       </c>
-      <c r="Q16" s="1">
+      <c r="Y16" s="1">
         <v>5557</v>
       </c>
-      <c r="R16" s="1">
+      <c r="Z16" s="1">
         <v>208</v>
       </c>
-      <c r="S16" s="1">
+      <c r="AA16" s="1">
         <v>11864</v>
       </c>
-      <c r="T16" s="1">
+      <c r="AB16" s="1">
         <v>1940</v>
       </c>
-      <c r="U16" s="1">
+      <c r="AC16" s="1">
         <v>220</v>
       </c>
-      <c r="V16" s="1">
+      <c r="AD16" s="1">
         <v>3434</v>
       </c>
-      <c r="W16" s="1">
+      <c r="AE16" s="1">
         <v>1234</v>
       </c>
-      <c r="X16" s="1">
+      <c r="AF16" s="1">
         <v>2628</v>
       </c>
-      <c r="Y16" s="1">
+      <c r="AG16" s="1">
         <v>105</v>
       </c>
-      <c r="Z16" s="1">
+      <c r="AH16" s="1">
         <v>4007</v>
       </c>
-      <c r="AA16" s="1">
+      <c r="AI16" s="1">
         <v>265</v>
       </c>
-      <c r="AB16" s="1">
+      <c r="AJ16" s="1">
         <v>11545</v>
       </c>
-      <c r="AC16" s="1">
+      <c r="AK16" s="1">
         <v>2350</v>
       </c>
-      <c r="AD16" s="1">
+      <c r="AL16" s="1">
         <v>274</v>
       </c>
-      <c r="AE16" s="1">
+      <c r="AM16" s="1">
         <v>3950</v>
       </c>
-      <c r="AF16" s="1">
+      <c r="AN16" s="1">
         <v>1634</v>
       </c>
-      <c r="AG16" s="1">
+      <c r="AO16" s="1">
         <v>2649</v>
       </c>
-      <c r="AH16" s="1">
+      <c r="AP16" s="1">
         <v>171</v>
       </c>
-      <c r="AI16" s="1">
+      <c r="AQ16" s="1">
         <v>305</v>
       </c>
-      <c r="AJ16" s="1">
+      <c r="AR16" s="1">
         <v>294</v>
       </c>
-      <c r="AK16" s="1">
+      <c r="AS16" s="1">
         <v>10630</v>
       </c>
-      <c r="AL16" s="1">
+      <c r="AT16" s="1">
         <v>2269</v>
       </c>
-      <c r="AM16" s="1">
+      <c r="AU16" s="1">
         <v>350</v>
       </c>
-      <c r="AN16" s="1">
+      <c r="AV16" s="1">
         <v>3611</v>
       </c>
-      <c r="AO16" s="1">
+      <c r="AW16" s="1">
         <v>1865</v>
       </c>
-      <c r="AP16" s="1">
+      <c r="AX16" s="1">
         <v>2690</v>
       </c>
-      <c r="AQ16" s="1">
+      <c r="AY16" s="1">
         <v>172</v>
       </c>
-      <c r="AR16" s="1">
+      <c r="AZ16" s="1">
         <v>534</v>
       </c>
-      <c r="AS16" s="1">
+      <c r="BA16" s="1">
         <v>10612</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C17" s="1">
+        <v>13159</v>
+      </c>
+      <c r="D17" s="1">
+        <v>5456</v>
+      </c>
+      <c r="E17" s="1">
+        <v>5481</v>
+      </c>
+      <c r="F17" s="1">
+        <v>3718</v>
+      </c>
+      <c r="G17" s="1">
+        <v>3767</v>
+      </c>
+      <c r="H17" s="1">
+        <v>417</v>
+      </c>
+      <c r="I17" s="1">
+        <v>812</v>
+      </c>
+      <c r="J17" s="1">
+        <v>28673</v>
+      </c>
+      <c r="K17" s="1">
         <v>11861</v>
       </c>
-      <c r="D17" s="1">
+      <c r="L17" s="1">
         <v>5398</v>
       </c>
-      <c r="E17" s="1">
+      <c r="M17" s="1">
         <v>5522</v>
       </c>
-      <c r="F17" s="1">
+      <c r="N17" s="1">
         <v>3898</v>
       </c>
-      <c r="G17" s="1">
+      <c r="O17" s="1">
         <v>4110</v>
       </c>
-      <c r="H17" s="1">
+      <c r="P17" s="1">
         <v>356</v>
       </c>
-      <c r="I17" s="1">
+      <c r="Q17" s="1">
         <v>1099</v>
       </c>
-      <c r="J17" s="1">
+      <c r="R17" s="1">
         <v>28650</v>
       </c>
-      <c r="K17" s="1">
+      <c r="S17" s="1">
         <v>10137</v>
       </c>
-      <c r="L17" s="1">
+      <c r="T17" s="1">
         <v>3736</v>
       </c>
-      <c r="M17" s="1">
+      <c r="U17" s="1">
         <v>5167</v>
       </c>
-      <c r="N17" s="1">
+      <c r="V17" s="1">
         <v>3005</v>
       </c>
-      <c r="O17" s="1">
+      <c r="W17" s="1">
         <v>3196</v>
       </c>
-      <c r="P17" s="1">
+      <c r="X17" s="1">
         <v>424</v>
       </c>
-      <c r="Q17" s="1">
+      <c r="Y17" s="1">
         <v>20425</v>
       </c>
-      <c r="R17" s="1">
+      <c r="Z17" s="1">
         <v>785</v>
       </c>
-      <c r="S17" s="1">
+      <c r="AA17" s="1">
         <v>38484</v>
       </c>
-      <c r="T17" s="1">
+      <c r="AB17" s="1">
         <v>10406</v>
       </c>
-      <c r="U17" s="1">
+      <c r="AC17" s="1">
         <v>5419</v>
       </c>
-      <c r="V17" s="1">
+      <c r="AD17" s="1">
         <v>5673</v>
       </c>
-      <c r="W17" s="1">
+      <c r="AE17" s="1">
         <v>3266</v>
       </c>
-      <c r="X17" s="1">
+      <c r="AF17" s="1">
         <v>3245</v>
       </c>
-      <c r="Y17" s="1">
+      <c r="AG17" s="1">
         <v>384</v>
       </c>
-      <c r="Z17" s="1">
+      <c r="AH17" s="1">
         <v>11993</v>
       </c>
-      <c r="AA17" s="1">
+      <c r="AI17" s="1">
         <v>801</v>
       </c>
-      <c r="AB17" s="1">
+      <c r="AJ17" s="1">
         <v>35267</v>
       </c>
-      <c r="AC17" s="1">
+      <c r="AK17" s="1">
         <v>10633</v>
       </c>
-      <c r="AD17" s="1">
+      <c r="AL17" s="1">
         <v>6109</v>
       </c>
-      <c r="AE17" s="1">
+      <c r="AM17" s="1">
         <v>6139</v>
       </c>
-      <c r="AF17" s="1">
+      <c r="AN17" s="1">
         <v>4276</v>
       </c>
-      <c r="AG17" s="1">
+      <c r="AO17" s="1">
         <v>3272</v>
       </c>
-      <c r="AH17" s="1">
+      <c r="AP17" s="1">
         <v>503</v>
       </c>
-      <c r="AI17" s="1">
+      <c r="AQ17" s="1">
         <v>619</v>
       </c>
-      <c r="AJ17" s="1">
+      <c r="AR17" s="1">
         <v>936</v>
       </c>
-      <c r="AK17" s="1">
+      <c r="AS17" s="1">
         <v>30297</v>
       </c>
-      <c r="AL17" s="1">
+      <c r="AT17" s="1">
         <v>9739</v>
       </c>
-      <c r="AM17" s="1">
+      <c r="AU17" s="1">
         <v>7318</v>
       </c>
-      <c r="AN17" s="1">
+      <c r="AV17" s="1">
         <v>5754</v>
       </c>
-      <c r="AO17" s="1">
+      <c r="AW17" s="1">
         <v>4619</v>
       </c>
-      <c r="AP17" s="1">
+      <c r="AX17" s="1">
         <v>3199</v>
       </c>
-      <c r="AQ17" s="1">
+      <c r="AY17" s="1">
         <v>514</v>
       </c>
-      <c r="AR17" s="1">
+      <c r="AZ17" s="1">
         <v>1324</v>
       </c>
-      <c r="AS17" s="1">
+      <c r="BA17" s="1">
         <v>30684</v>
       </c>
     </row>
@@ -2101,11 +2421,12 @@
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="C5:J5"/>
-    <mergeCell ref="K5:S5"/>
-    <mergeCell ref="T5:AB5"/>
-    <mergeCell ref="AC5:AK5"/>
-    <mergeCell ref="AL5:AS5"/>
-    <mergeCell ref="C7:AS7"/>
+    <mergeCell ref="K5:R5"/>
+    <mergeCell ref="S5:AA5"/>
+    <mergeCell ref="AB5:AJ5"/>
+    <mergeCell ref="AK5:AS5"/>
+    <mergeCell ref="AT5:BA5"/>
+    <mergeCell ref="C7:BA7"/>
     <mergeCell ref="A10:A17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>